<commit_message>
Project Plan for now
</commit_message>
<xml_diff>
--- a/Documents/GanttChart_EquifoodA.xlsx
+++ b/Documents/GanttChart_EquifoodA.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2260B18-D322-4FDF-984F-9A79F2EC5F46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A35E1621-6822-4C05-9433-CCCD444E1792}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="68">
   <si>
     <t>Task 3</t>
   </si>
@@ -260,6 +260,26 @@
   </si>
   <si>
     <t>Backend: Create User DB</t>
+  </si>
+  <si>
+    <t>Converting project from Ionic React into React Native</t>
+  </si>
+  <si>
+    <t>Amrita</t>
+  </si>
+  <si>
+    <t>Implementing / improving UI features on Web and
+Mobile once Jake converts</t>
+  </si>
+  <si>
+    <t>Code to allow to app to fetch all data in real time from
+database.</t>
+  </si>
+  <si>
+    <t>Backend for restaurant rep to insert data to database</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Abhiek </t>
   </si>
 </sst>
 </file>
@@ -639,7 +659,7 @@
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="83">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -855,6 +875,12 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="1" applyFont="1" applyProtection="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="8">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="8" applyBorder="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
     <xf numFmtId="167" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -867,11 +893,8 @@
     <xf numFmtId="166" fontId="9" fillId="0" borderId="3" xfId="9">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="8">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="8" applyBorder="1">
-      <alignment horizontal="right" indent="1"/>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="2" xfId="12" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
     </xf>
   </cellXfs>
   <cellStyles count="13">
@@ -1386,14 +1409,14 @@
   <dimension ref="A1:BL47"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="101" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B20" sqref="B20"/>
+      <pane ySplit="6" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="2.6328125" style="48" customWidth="1"/>
-    <col min="2" max="2" width="36.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="48.08984375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="30.6328125" customWidth="1"/>
     <col min="4" max="4" width="10.6328125" customWidth="1"/>
     <col min="5" max="5" width="10.453125" style="5" customWidth="1"/>
@@ -1430,106 +1453,106 @@
         <v>26</v>
       </c>
       <c r="B3" s="54"/>
-      <c r="C3" s="81" t="s">
+      <c r="C3" s="77" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="82"/>
-      <c r="E3" s="80">
+      <c r="D3" s="78"/>
+      <c r="E3" s="82">
         <v>44841</v>
       </c>
-      <c r="F3" s="80"/>
+      <c r="F3" s="82"/>
     </row>
     <row r="4" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="49" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="81" t="s">
+      <c r="C4" s="77" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="82"/>
+      <c r="D4" s="78"/>
       <c r="E4" s="7">
         <v>1</v>
       </c>
-      <c r="I4" s="77">
+      <c r="I4" s="79">
         <f>I5</f>
         <v>44837</v>
       </c>
-      <c r="J4" s="78"/>
-      <c r="K4" s="78"/>
-      <c r="L4" s="78"/>
-      <c r="M4" s="78"/>
-      <c r="N4" s="78"/>
-      <c r="O4" s="79"/>
-      <c r="P4" s="77">
+      <c r="J4" s="80"/>
+      <c r="K4" s="80"/>
+      <c r="L4" s="80"/>
+      <c r="M4" s="80"/>
+      <c r="N4" s="80"/>
+      <c r="O4" s="81"/>
+      <c r="P4" s="79">
         <f>P5</f>
         <v>44844</v>
       </c>
-      <c r="Q4" s="78"/>
-      <c r="R4" s="78"/>
-      <c r="S4" s="78"/>
-      <c r="T4" s="78"/>
-      <c r="U4" s="78"/>
-      <c r="V4" s="79"/>
-      <c r="W4" s="77">
+      <c r="Q4" s="80"/>
+      <c r="R4" s="80"/>
+      <c r="S4" s="80"/>
+      <c r="T4" s="80"/>
+      <c r="U4" s="80"/>
+      <c r="V4" s="81"/>
+      <c r="W4" s="79">
         <f>W5</f>
         <v>44851</v>
       </c>
-      <c r="X4" s="78"/>
-      <c r="Y4" s="78"/>
-      <c r="Z4" s="78"/>
-      <c r="AA4" s="78"/>
-      <c r="AB4" s="78"/>
-      <c r="AC4" s="79"/>
-      <c r="AD4" s="77">
+      <c r="X4" s="80"/>
+      <c r="Y4" s="80"/>
+      <c r="Z4" s="80"/>
+      <c r="AA4" s="80"/>
+      <c r="AB4" s="80"/>
+      <c r="AC4" s="81"/>
+      <c r="AD4" s="79">
         <f>AD5</f>
         <v>44858</v>
       </c>
-      <c r="AE4" s="78"/>
-      <c r="AF4" s="78"/>
-      <c r="AG4" s="78"/>
-      <c r="AH4" s="78"/>
-      <c r="AI4" s="78"/>
-      <c r="AJ4" s="79"/>
-      <c r="AK4" s="77">
+      <c r="AE4" s="80"/>
+      <c r="AF4" s="80"/>
+      <c r="AG4" s="80"/>
+      <c r="AH4" s="80"/>
+      <c r="AI4" s="80"/>
+      <c r="AJ4" s="81"/>
+      <c r="AK4" s="79">
         <f>AK5</f>
         <v>44865</v>
       </c>
-      <c r="AL4" s="78"/>
-      <c r="AM4" s="78"/>
-      <c r="AN4" s="78"/>
-      <c r="AO4" s="78"/>
-      <c r="AP4" s="78"/>
-      <c r="AQ4" s="79"/>
-      <c r="AR4" s="77">
+      <c r="AL4" s="80"/>
+      <c r="AM4" s="80"/>
+      <c r="AN4" s="80"/>
+      <c r="AO4" s="80"/>
+      <c r="AP4" s="80"/>
+      <c r="AQ4" s="81"/>
+      <c r="AR4" s="79">
         <f>AR5</f>
         <v>44872</v>
       </c>
-      <c r="AS4" s="78"/>
-      <c r="AT4" s="78"/>
-      <c r="AU4" s="78"/>
-      <c r="AV4" s="78"/>
-      <c r="AW4" s="78"/>
-      <c r="AX4" s="79"/>
-      <c r="AY4" s="77">
+      <c r="AS4" s="80"/>
+      <c r="AT4" s="80"/>
+      <c r="AU4" s="80"/>
+      <c r="AV4" s="80"/>
+      <c r="AW4" s="80"/>
+      <c r="AX4" s="81"/>
+      <c r="AY4" s="79">
         <f>AY5</f>
         <v>44879</v>
       </c>
-      <c r="AZ4" s="78"/>
-      <c r="BA4" s="78"/>
-      <c r="BB4" s="78"/>
-      <c r="BC4" s="78"/>
-      <c r="BD4" s="78"/>
-      <c r="BE4" s="79"/>
-      <c r="BF4" s="77">
+      <c r="AZ4" s="80"/>
+      <c r="BA4" s="80"/>
+      <c r="BB4" s="80"/>
+      <c r="BC4" s="80"/>
+      <c r="BD4" s="80"/>
+      <c r="BE4" s="81"/>
+      <c r="BF4" s="79">
         <f>BF5</f>
         <v>44886</v>
       </c>
-      <c r="BG4" s="78"/>
-      <c r="BH4" s="78"/>
-      <c r="BI4" s="78"/>
-      <c r="BJ4" s="78"/>
-      <c r="BK4" s="78"/>
-      <c r="BL4" s="79"/>
+      <c r="BG4" s="80"/>
+      <c r="BH4" s="80"/>
+      <c r="BI4" s="80"/>
+      <c r="BJ4" s="80"/>
+      <c r="BK4" s="80"/>
+      <c r="BL4" s="81"/>
     </row>
     <row r="5" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="49" t="s">
@@ -2871,7 +2894,7 @@
         <v>35</v>
       </c>
       <c r="D18" s="27">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="E18" s="56">
         <v>44860</v>
@@ -3924,22 +3947,23 @@
     <row r="32" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A32" s="48"/>
       <c r="B32" s="71" t="s">
-        <v>3</v>
-      </c>
-      <c r="C32" s="65"/>
+        <v>62</v>
+      </c>
+      <c r="C32" s="65" t="s">
+        <v>54</v>
+      </c>
       <c r="D32" s="32"/>
       <c r="E32" s="57">
-        <f>E9+15</f>
-        <v>44856</v>
+        <v>44937</v>
       </c>
       <c r="F32" s="57">
-        <f>E32+5</f>
-        <v>44861</v>
+        <f>E32+4</f>
+        <v>44941</v>
       </c>
       <c r="G32" s="17"/>
       <c r="H32" s="17">
         <f t="shared" si="6"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I32" s="44"/>
       <c r="J32" s="44"/>
@@ -4000,18 +4024,20 @@
     </row>
     <row r="33" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A33" s="48"/>
-      <c r="B33" s="71" t="s">
-        <v>4</v>
-      </c>
-      <c r="C33" s="65"/>
+      <c r="B33" s="83" t="s">
+        <v>64</v>
+      </c>
+      <c r="C33" s="65" t="s">
+        <v>63</v>
+      </c>
       <c r="D33" s="32"/>
       <c r="E33" s="57">
         <f>F32+1</f>
-        <v>44862</v>
+        <v>44942</v>
       </c>
       <c r="F33" s="57">
         <f>E33+4</f>
-        <v>44866</v>
+        <v>44946</v>
       </c>
       <c r="G33" s="17"/>
       <c r="H33" s="17">
@@ -4077,23 +4103,24 @@
     </row>
     <row r="34" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A34" s="48"/>
-      <c r="B34" s="71" t="s">
-        <v>0</v>
-      </c>
-      <c r="C34" s="65"/>
+      <c r="B34" s="83" t="s">
+        <v>65</v>
+      </c>
+      <c r="C34" s="65" t="s">
+        <v>57</v>
+      </c>
       <c r="D34" s="32"/>
       <c r="E34" s="57">
-        <f>E33+5</f>
-        <v>44867</v>
+        <v>44937</v>
       </c>
       <c r="F34" s="57">
-        <f>E34+5</f>
-        <v>44872</v>
+        <f>E34+4</f>
+        <v>44941</v>
       </c>
       <c r="G34" s="17"/>
       <c r="H34" s="17">
         <f t="shared" si="6"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I34" s="44"/>
       <c r="J34" s="44"/>
@@ -4155,22 +4182,24 @@
     <row r="35" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A35" s="48"/>
       <c r="B35" s="71" t="s">
-        <v>1</v>
-      </c>
-      <c r="C35" s="65"/>
+        <v>66</v>
+      </c>
+      <c r="C35" s="65" t="s">
+        <v>67</v>
+      </c>
       <c r="D35" s="32"/>
       <c r="E35" s="57">
         <f>F34+1</f>
-        <v>44873</v>
+        <v>44942</v>
       </c>
       <c r="F35" s="57">
-        <f>E35+4</f>
-        <v>44877</v>
+        <f>E35+6</f>
+        <v>44948</v>
       </c>
       <c r="G35" s="17"/>
       <c r="H35" s="17">
         <f t="shared" si="6"/>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="I35" s="44"/>
       <c r="J35" s="44"/>
@@ -4238,11 +4267,11 @@
       <c r="D36" s="32"/>
       <c r="E36" s="57">
         <f>E34</f>
-        <v>44867</v>
+        <v>44937</v>
       </c>
       <c r="F36" s="57">
         <f>E36+4</f>
-        <v>44871</v>
+        <v>44941</v>
       </c>
       <c r="G36" s="17"/>
       <c r="H36" s="17">
@@ -4910,17 +4939,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="AK4:AQ4"/>
-    <mergeCell ref="AR4:AX4"/>
-    <mergeCell ref="AY4:BE4"/>
     <mergeCell ref="BF4:BL4"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="I4:O4"/>
     <mergeCell ref="P4:V4"/>
     <mergeCell ref="W4:AC4"/>
     <mergeCell ref="AD4:AJ4"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="AK4:AQ4"/>
+    <mergeCell ref="AR4:AX4"/>
+    <mergeCell ref="AY4:BE4"/>
   </mergeCells>
   <conditionalFormatting sqref="D7:D44">
     <cfRule type="dataBar" priority="14">
@@ -4961,7 +4990,7 @@
     <oddFooter>Page &amp;P of &amp;N</oddFooter>
   </headerFooter>
   <ignoredErrors>
-    <ignoredError sqref="F33:F34 E34" formula="1"/>
+    <ignoredError sqref="F33" formula="1"/>
   </ignoredErrors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">

</xml_diff>